<commit_message>
fixed diagram & sheets
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -927,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,13 +1255,13 @@
       <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="14" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1283,13 +1283,13 @@
       <c r="A12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="14" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1309,6 +1309,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>